<commit_message>
Debugging exe and accuracy
</commit_message>
<xml_diff>
--- a/Test Files/Test.xlsx
+++ b/Test Files/Test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="360" yWindow="360" windowWidth="19185" windowHeight="10185" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -24,8 +24,14 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -34,8 +40,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00F1EB9C"/>
-        <bgColor rgb="00F1EB9C"/>
+        <fgColor rgb="008FB547"/>
+        <bgColor rgb="008FB547"/>
       </patternFill>
     </fill>
     <fill>
@@ -44,14 +50,8 @@
         <bgColor rgb="0084C4E4"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="008FB547"/>
-        <bgColor rgb="008FB547"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -59,20 +59,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -464,16 +485,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.7109375" bestFit="1" customWidth="1" min="2" max="2"/>
     <col width="9.7109375" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="33.7109375" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -494,212 +516,118 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CMA </t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>CMAU1999430</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>Date Error</t>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>CMA</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>GESU5876310</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t>arrived</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>######6/26/2022#######</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CMA </t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>TEMU1001882</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>Date Error</t>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>CMA</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>CMAU8671334</t>
+        </is>
+      </c>
+      <c r="C3" s="6" t="inlineStr">
+        <is>
+          <t>06/25/2022</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>############6/25/2022##########</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CMA </t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>TRHU6017442</t>
-        </is>
-      </c>
-      <c r="C4" s="3" t="inlineStr">
-        <is>
-          <t>07/17/2022</t>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>CMA</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>CMAU5726794</t>
+        </is>
+      </c>
+      <c r="C4" s="6" t="inlineStr">
+        <is>
+          <t>07/01/2022</t>
+        </is>
+      </c>
+      <c r="E4" s="4" t="inlineStr">
+        <is>
+          <t>###########07/01/2022##########</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CMA </t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>JXLU7831639</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>Date Error</t>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>CMA</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>CMAU5875885</t>
+        </is>
+      </c>
+      <c r="C5" s="6" t="inlineStr">
+        <is>
+          <t>07/01/2022</t>
+        </is>
+      </c>
+      <c r="E5" s="4" t="inlineStr">
+        <is>
+          <t>#########07/01/2022############</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CMA </t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>DFSU6935165</t>
-        </is>
-      </c>
-      <c r="C6" s="3" t="inlineStr">
-        <is>
-          <t>07/25/2022</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CMA </t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>BMOU2183772</t>
-        </is>
-      </c>
-      <c r="C7" s="2" t="inlineStr">
-        <is>
-          <t>Date Error</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CMA </t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>BMOU2182267</t>
-        </is>
-      </c>
-      <c r="C8" s="4" t="inlineStr">
-        <is>
-          <t>arrived</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CMA </t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>CMAU7146898</t>
-        </is>
-      </c>
-      <c r="C9" s="4" t="inlineStr">
-        <is>
-          <t>arrived</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CMA </t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>FWRU0143517</t>
-        </is>
-      </c>
-      <c r="C10" s="4" t="inlineStr">
-        <is>
-          <t>arrived</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CMA </t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>TEMU2454266</t>
-        </is>
-      </c>
-      <c r="C11" s="4" t="inlineStr">
-        <is>
-          <t>arrived</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CMA </t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>CMAU0615186</t>
-        </is>
-      </c>
-      <c r="C12" s="4" t="inlineStr">
-        <is>
-          <t>arrived</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CMA </t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>CMAU1671749</t>
-        </is>
-      </c>
-      <c r="C13" s="4" t="inlineStr">
-        <is>
-          <t>arrived</t>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>CMA</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>TCKU6228690</t>
+        </is>
+      </c>
+      <c r="C6" s="6" t="inlineStr">
+        <is>
+          <t>07/06/2022</t>
+        </is>
+      </c>
+      <c r="E6" s="4" t="inlineStr">
+        <is>
+          <t>############07/06/2022##########</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B13">
-    <cfRule type="duplicateValues" priority="3" dxfId="0"/>
+  <conditionalFormatting sqref="B1">
+    <cfRule type="duplicateValues" priority="4" dxfId="0"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>